<commit_message>
Semana 2 sin cambios, semana 3 cambios parciales.
</commit_message>
<xml_diff>
--- a/Horario.xlsx
+++ b/Horario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA00199-3503-4FE2-954B-81E16D385BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099B7CA0-691A-4632-852B-93026872F3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{5BBD8727-8E97-4145-910C-D98B6570B875}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="35">
   <si>
     <t>Semana 1 (Febrero 13 - Febrero 19)</t>
   </si>
@@ -135,13 +135,19 @@
   </si>
   <si>
     <t>CITA MEDICA</t>
+  </si>
+  <si>
+    <t>QUIZ #1 CALCULO</t>
+  </si>
+  <si>
+    <t>CITA OPTOMETRÍA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +178,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -251,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -439,11 +452,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -464,16 +516,61 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -488,115 +585,95 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -607,8 +684,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FF66"/>
+      <color rgb="FFC9E7A7"/>
       <color rgb="FFFF5050"/>
-      <color rgb="FF99FF66"/>
       <color rgb="FF66FFFF"/>
     </mruColors>
   </colors>
@@ -922,111 +1000,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BDC904-63CB-49D9-B79D-E95CC9E732E1}">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46:M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
     </row>
     <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A2" s="9"/>
       <c r="B2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="38"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="39"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="39"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
+      <c r="I2" s="38"/>
       <c r="J2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="39"/>
+      <c r="K2" s="38"/>
       <c r="L2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="39"/>
+      <c r="M2" s="38"/>
       <c r="N2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="39"/>
+      <c r="O2" s="38"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="26" t="s">
+      <c r="B3" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="26" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="34"/>
+      <c r="H3" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="27"/>
+      <c r="I3" s="42"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
-      <c r="L3" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="19"/>
+      <c r="L3" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="34"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="21"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="36"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
@@ -1034,20 +1112,20 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="26" t="s">
+      <c r="I5" s="52"/>
+      <c r="J5" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="27"/>
+      <c r="K5" s="42"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
@@ -1059,14 +1137,14 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="54"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="29"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="46"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
@@ -1078,18 +1156,18 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="33"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="33"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="31"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="44"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
@@ -1101,12 +1179,12 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="35"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="58"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="10"/>
@@ -1118,64 +1196,64 @@
       <c r="A9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="48"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="48" t="s">
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="49"/>
+      <c r="O9" s="26"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="51"/>
+      <c r="J10" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="34"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="28"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="19"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="34"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="21"/>
+      <c r="H11" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="34"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="36"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
       <c r="N11" s="10"/>
@@ -1187,12 +1265,12 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -1231,10 +1309,10 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="15"/>
+      <c r="K14" s="48"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
@@ -1244,22 +1322,22 @@
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="15"/>
+      <c r="E15" s="48"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="17"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="50"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
@@ -1269,14 +1347,14 @@
       <c r="A16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="50"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="17"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="10"/>
@@ -1318,127 +1396,127 @@
       <c r="O18" s="1"/>
     </row>
     <row r="21" spans="1:16" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
     </row>
     <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A22" s="9"/>
       <c r="B22" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="38"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="39"/>
+      <c r="E22" s="38"/>
       <c r="F22" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="39"/>
+      <c r="G22" s="38"/>
       <c r="H22" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="39"/>
+      <c r="I22" s="38"/>
       <c r="J22" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="K22" s="39"/>
+      <c r="K22" s="38"/>
       <c r="L22" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="M22" s="39"/>
+      <c r="M22" s="38"/>
       <c r="N22" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="O22" s="39"/>
+      <c r="O22" s="38"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="26" t="s">
+      <c r="B23" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="27"/>
-      <c r="F23" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="26" t="s">
+      <c r="E23" s="42"/>
+      <c r="F23" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="34"/>
+      <c r="H23" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="27"/>
+      <c r="I23" s="42"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
-      <c r="L23" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="M23" s="19"/>
-      <c r="N23" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="O23" s="19"/>
+      <c r="L23" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="34"/>
+      <c r="N23" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="O23" s="34"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="31"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="44"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="21"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="36"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="22" t="s">
+      <c r="C25" s="22"/>
+      <c r="D25" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="23"/>
+      <c r="E25" s="52"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="26" t="s">
+      <c r="I25" s="52"/>
+      <c r="J25" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="K25" s="27"/>
+      <c r="K25" s="42"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
@@ -1448,16 +1526,16 @@
       <c r="A26" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="54"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="29"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="46"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
@@ -1469,18 +1547,18 @@
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="33"/>
+      <c r="E27" s="56"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="32" t="s">
+      <c r="H27" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="I27" s="33"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="31"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="44"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
@@ -1492,12 +1570,12 @@
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="35"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="58"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="35"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="59"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="10"/>
@@ -1509,24 +1587,24 @@
       <c r="A29" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="48"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="10"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="61"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
-      <c r="L29" s="14" t="s">
+      <c r="L29" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="15"/>
+      <c r="M29" s="48"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
     </row>
@@ -1534,20 +1612,20 @@
       <c r="A30" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="17"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="50"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
-      <c r="J30" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K30" s="19"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="17"/>
+      <c r="J30" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K30" s="34"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="50"/>
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
     </row>
@@ -1557,18 +1635,18 @@
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
-      <c r="D31" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="19"/>
+      <c r="D31" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="34"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
-      <c r="H31" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I31" s="19"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="21"/>
+      <c r="H31" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" s="34"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="36"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
       <c r="N31" s="10"/>
@@ -1580,12 +1658,12 @@
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="21"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="36"/>
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
       <c r="L32" s="10"/>
@@ -1624,10 +1702,10 @@
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
-      <c r="J34" s="14" t="s">
+      <c r="J34" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="K34" s="15"/>
+      <c r="K34" s="48"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
@@ -1639,18 +1717,18 @@
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="15"/>
+      <c r="E35" s="48"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
-      <c r="H35" s="14" t="s">
+      <c r="H35" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I35" s="15"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="17"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="50"/>
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
@@ -1662,12 +1740,12 @@
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="17"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="50"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="17"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="50"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="10"/>
@@ -1676,104 +1754,104 @@
       <c r="O36" s="10"/>
     </row>
     <row r="41" spans="1:15" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
-      <c r="O41" s="36"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="39"/>
+      <c r="M41" s="39"/>
+      <c r="N41" s="39"/>
+      <c r="O41" s="39"/>
     </row>
     <row r="42" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A42" s="9"/>
       <c r="B42" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="38"/>
+      <c r="C42" s="40"/>
       <c r="D42" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="39"/>
+      <c r="E42" s="38"/>
       <c r="F42" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G42" s="39"/>
+      <c r="G42" s="38"/>
       <c r="H42" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I42" s="39"/>
+      <c r="I42" s="38"/>
       <c r="J42" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="K42" s="39"/>
+      <c r="K42" s="38"/>
       <c r="L42" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="M42" s="39"/>
+      <c r="M42" s="38"/>
       <c r="N42" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="O42" s="39"/>
+      <c r="O42" s="38"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="26" t="s">
+      <c r="B43" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="34"/>
+      <c r="D43" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G43" s="19"/>
-      <c r="H43" s="26" t="s">
+      <c r="E43" s="42"/>
+      <c r="F43" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="34"/>
+      <c r="H43" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I43" s="27"/>
+      <c r="I43" s="42"/>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
-      <c r="L43" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="M43" s="19"/>
-      <c r="N43" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="O43" s="19"/>
+      <c r="L43" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="M43" s="34"/>
+      <c r="N43" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="O43" s="34"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="31"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="44"/>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="21"/>
-      <c r="N44" s="20"/>
-      <c r="O44" s="21"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="36"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="36"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
@@ -1781,20 +1859,20 @@
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="E45" s="23"/>
+      <c r="E45" s="52"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I45" s="23"/>
-      <c r="J45" s="26" t="s">
+      <c r="I45" s="52"/>
+      <c r="J45" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="K45" s="27"/>
+      <c r="K45" s="42"/>
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
@@ -1806,16 +1884,18 @@
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="25"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="54"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="10"/>
-      <c r="M46" s="10"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="54"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="M46" s="65"/>
       <c r="N46" s="10"/>
       <c r="O46" s="10"/>
     </row>
@@ -1825,20 +1905,20 @@
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
-      <c r="D47" s="32" t="s">
+      <c r="D47" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E47" s="33"/>
+      <c r="E47" s="56"/>
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
-      <c r="H47" s="32" t="s">
+      <c r="H47" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="I47" s="33"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="10"/>
-      <c r="M47" s="10"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="66"/>
+      <c r="M47" s="67"/>
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
     </row>
@@ -1848,12 +1928,12 @@
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="35"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="58"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="35"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="58"/>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="10"/>
@@ -1865,24 +1945,24 @@
       <c r="A49" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="15"/>
+      <c r="C49" s="48"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
-      <c r="F49" s="14" t="s">
+      <c r="F49" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="G49" s="15"/>
+      <c r="G49" s="48"/>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
-      <c r="L49" s="14" t="s">
+      <c r="L49" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="M49" s="15"/>
+      <c r="M49" s="48"/>
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
     </row>
@@ -1890,20 +1970,20 @@
       <c r="A50" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="17"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="50"/>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="17"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="50"/>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
-      <c r="J50" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K50" s="19"/>
-      <c r="L50" s="16"/>
-      <c r="M50" s="17"/>
+      <c r="J50" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K50" s="34"/>
+      <c r="L50" s="49"/>
+      <c r="M50" s="50"/>
       <c r="N50" s="10"/>
       <c r="O50" s="10"/>
     </row>
@@ -1913,18 +1993,18 @@
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
-      <c r="D51" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="19"/>
+      <c r="D51" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" s="34"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
-      <c r="H51" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I51" s="19"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="21"/>
+      <c r="H51" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I51" s="34"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="36"/>
       <c r="L51" s="12"/>
       <c r="M51" s="12"/>
       <c r="N51" s="10"/>
@@ -1936,12 +2016,12 @@
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="21"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="36"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="21"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="36"/>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
@@ -1959,8 +2039,10 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
+      <c r="H53" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="I53" s="52"/>
       <c r="J53" s="10"/>
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
@@ -1978,12 +2060,12 @@
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="10"/>
-      <c r="J54" s="14" t="s">
+      <c r="H54" s="53"/>
+      <c r="I54" s="54"/>
+      <c r="J54" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="K54" s="15"/>
+      <c r="K54" s="48"/>
       <c r="L54" s="10"/>
       <c r="M54" s="10"/>
       <c r="N54" s="10"/>
@@ -1995,18 +2077,18 @@
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="15"/>
+      <c r="E55" s="48"/>
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
-      <c r="H55" s="14" t="s">
+      <c r="H55" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I55" s="15"/>
-      <c r="J55" s="16"/>
-      <c r="K55" s="17"/>
+      <c r="I55" s="48"/>
+      <c r="J55" s="49"/>
+      <c r="K55" s="50"/>
       <c r="L55" s="10"/>
       <c r="M55" s="10"/>
       <c r="N55" s="10"/>
@@ -2018,12 +2100,12 @@
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="17"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="50"/>
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="17"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="50"/>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="10"/>
@@ -2032,104 +2114,104 @@
       <c r="O56" s="10"/>
     </row>
     <row r="61" spans="1:15" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A61" s="36" t="s">
+      <c r="A61" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="36"/>
-      <c r="K61" s="36"/>
-      <c r="L61" s="36"/>
-      <c r="M61" s="36"/>
-      <c r="N61" s="36"/>
-      <c r="O61" s="36"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="39"/>
+      <c r="J61" s="39"/>
+      <c r="K61" s="39"/>
+      <c r="L61" s="39"/>
+      <c r="M61" s="39"/>
+      <c r="N61" s="39"/>
+      <c r="O61" s="39"/>
     </row>
     <row r="62" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A62" s="9"/>
       <c r="B62" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="38"/>
+      <c r="C62" s="40"/>
       <c r="D62" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="39"/>
+      <c r="E62" s="38"/>
       <c r="F62" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G62" s="39"/>
+      <c r="G62" s="38"/>
       <c r="H62" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I62" s="39"/>
+      <c r="I62" s="38"/>
       <c r="J62" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="K62" s="39"/>
+      <c r="K62" s="38"/>
       <c r="L62" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="M62" s="39"/>
+      <c r="M62" s="38"/>
       <c r="N62" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="O62" s="39"/>
+      <c r="O62" s="38"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B63" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="19"/>
-      <c r="D63" s="26" t="s">
+      <c r="B63" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="34"/>
+      <c r="D63" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E63" s="27"/>
-      <c r="F63" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G63" s="19"/>
-      <c r="H63" s="26" t="s">
+      <c r="E63" s="42"/>
+      <c r="F63" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G63" s="34"/>
+      <c r="H63" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I63" s="27"/>
+      <c r="I63" s="42"/>
       <c r="J63" s="10"/>
       <c r="K63" s="10"/>
-      <c r="L63" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="M63" s="19"/>
-      <c r="N63" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="O63" s="19"/>
+      <c r="L63" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="M63" s="34"/>
+      <c r="N63" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="O63" s="34"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B64" s="20"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="31"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="21"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="31"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="44"/>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
-      <c r="L64" s="20"/>
-      <c r="M64" s="21"/>
-      <c r="N64" s="20"/>
-      <c r="O64" s="21"/>
+      <c r="L64" s="35"/>
+      <c r="M64" s="36"/>
+      <c r="N64" s="35"/>
+      <c r="O64" s="36"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
@@ -2137,20 +2219,20 @@
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
-      <c r="D65" s="22" t="s">
+      <c r="D65" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="E65" s="23"/>
+      <c r="E65" s="52"/>
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
-      <c r="H65" s="22" t="s">
+      <c r="H65" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="I65" s="23"/>
-      <c r="J65" s="26" t="s">
+      <c r="I65" s="52"/>
+      <c r="J65" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="K65" s="27"/>
+      <c r="K65" s="42"/>
       <c r="L65" s="10"/>
       <c r="M65" s="10"/>
       <c r="N65" s="10"/>
@@ -2162,14 +2244,14 @@
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="25"/>
+      <c r="D66" s="53"/>
+      <c r="E66" s="54"/>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
-      <c r="H66" s="24"/>
-      <c r="I66" s="25"/>
-      <c r="J66" s="28"/>
-      <c r="K66" s="29"/>
+      <c r="H66" s="53"/>
+      <c r="I66" s="54"/>
+      <c r="J66" s="45"/>
+      <c r="K66" s="46"/>
       <c r="L66" s="10"/>
       <c r="M66" s="10"/>
       <c r="N66" s="10"/>
@@ -2181,18 +2263,15 @@
       </c>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
-      <c r="D67" s="32" t="s">
+      <c r="D67" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E67" s="33"/>
+      <c r="E67" s="56"/>
       <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
-      <c r="H67" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="I67" s="33"/>
-      <c r="J67" s="30"/>
-      <c r="K67" s="31"/>
+      <c r="G67" s="14"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="43"/>
+      <c r="K67" s="44"/>
       <c r="L67" s="10"/>
       <c r="M67" s="10"/>
       <c r="N67" s="10"/>
@@ -2204,12 +2283,12 @@
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
-      <c r="D68" s="34"/>
-      <c r="E68" s="35"/>
+      <c r="D68" s="57"/>
+      <c r="E68" s="58"/>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
-      <c r="H68" s="34"/>
-      <c r="I68" s="35"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="17"/>
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
       <c r="L68" s="10"/>
@@ -2221,24 +2300,24 @@
       <c r="A69" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C69" s="15"/>
+      <c r="C69" s="48"/>
       <c r="D69" s="10"/>
       <c r="E69" s="10"/>
-      <c r="F69" s="14" t="s">
+      <c r="F69" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="G69" s="15"/>
+      <c r="G69" s="48"/>
       <c r="H69" s="10"/>
       <c r="I69" s="10"/>
       <c r="J69" s="10"/>
       <c r="K69" s="10"/>
-      <c r="L69" s="14" t="s">
+      <c r="L69" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="M69" s="15"/>
+      <c r="M69" s="48"/>
       <c r="N69" s="10"/>
       <c r="O69" s="10"/>
     </row>
@@ -2246,20 +2325,20 @@
       <c r="A70" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B70" s="16"/>
-      <c r="C70" s="17"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="50"/>
       <c r="D70" s="10"/>
       <c r="E70" s="10"/>
-      <c r="F70" s="16"/>
-      <c r="G70" s="17"/>
+      <c r="F70" s="49"/>
+      <c r="G70" s="50"/>
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
-      <c r="J70" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K70" s="19"/>
-      <c r="L70" s="16"/>
-      <c r="M70" s="17"/>
+      <c r="J70" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K70" s="34"/>
+      <c r="L70" s="49"/>
+      <c r="M70" s="50"/>
       <c r="N70" s="10"/>
       <c r="O70" s="10"/>
     </row>
@@ -2269,18 +2348,18 @@
       </c>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
-      <c r="D71" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E71" s="19"/>
+      <c r="D71" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" s="34"/>
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
-      <c r="H71" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I71" s="19"/>
-      <c r="J71" s="20"/>
-      <c r="K71" s="21"/>
+      <c r="H71" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I71" s="34"/>
+      <c r="J71" s="35"/>
+      <c r="K71" s="36"/>
       <c r="L71" s="12"/>
       <c r="M71" s="12"/>
       <c r="N71" s="10"/>
@@ -2292,12 +2371,12 @@
       </c>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="21"/>
+      <c r="D72" s="35"/>
+      <c r="E72" s="36"/>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
-      <c r="H72" s="20"/>
-      <c r="I72" s="21"/>
+      <c r="H72" s="35"/>
+      <c r="I72" s="36"/>
       <c r="J72" s="10"/>
       <c r="K72" s="10"/>
       <c r="L72" s="10"/>
@@ -2336,10 +2415,10 @@
       <c r="G74" s="10"/>
       <c r="H74" s="10"/>
       <c r="I74" s="10"/>
-      <c r="J74" s="14" t="s">
+      <c r="J74" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="K74" s="15"/>
+      <c r="K74" s="48"/>
       <c r="L74" s="10"/>
       <c r="M74" s="10"/>
       <c r="N74" s="10"/>
@@ -2351,18 +2430,18 @@
       </c>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
-      <c r="D75" s="14" t="s">
+      <c r="D75" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="15"/>
+      <c r="E75" s="48"/>
       <c r="F75" s="11"/>
       <c r="G75" s="11"/>
-      <c r="H75" s="14" t="s">
+      <c r="H75" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I75" s="15"/>
-      <c r="J75" s="16"/>
-      <c r="K75" s="17"/>
+      <c r="I75" s="48"/>
+      <c r="J75" s="49"/>
+      <c r="K75" s="50"/>
       <c r="L75" s="10"/>
       <c r="M75" s="10"/>
       <c r="N75" s="10"/>
@@ -2374,12 +2453,12 @@
       </c>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
-      <c r="D76" s="16"/>
-      <c r="E76" s="17"/>
+      <c r="D76" s="49"/>
+      <c r="E76" s="50"/>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
-      <c r="H76" s="16"/>
-      <c r="I76" s="17"/>
+      <c r="H76" s="49"/>
+      <c r="I76" s="50"/>
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
       <c r="L76" s="10"/>
@@ -2389,27 +2468,74 @@
     </row>
   </sheetData>
   <mergeCells count="113">
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="N9:O10"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="J10:K11"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="H11:I12"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="J5:K7"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="H15:I16"/>
-    <mergeCell ref="J14:K15"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="L69:M70"/>
+    <mergeCell ref="J70:K71"/>
+    <mergeCell ref="D71:E72"/>
+    <mergeCell ref="H71:I72"/>
+    <mergeCell ref="J74:K75"/>
+    <mergeCell ref="D75:E76"/>
+    <mergeCell ref="H75:I76"/>
+    <mergeCell ref="D65:E66"/>
+    <mergeCell ref="H65:I66"/>
+    <mergeCell ref="J65:K67"/>
+    <mergeCell ref="D67:E68"/>
+    <mergeCell ref="L63:M64"/>
+    <mergeCell ref="N63:O64"/>
+    <mergeCell ref="A61:O61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="J54:K55"/>
+    <mergeCell ref="D55:E56"/>
+    <mergeCell ref="H55:I56"/>
+    <mergeCell ref="D45:E46"/>
+    <mergeCell ref="H45:I46"/>
+    <mergeCell ref="J45:K47"/>
+    <mergeCell ref="D47:E48"/>
+    <mergeCell ref="H47:I48"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="F69:G70"/>
+    <mergeCell ref="B63:C64"/>
+    <mergeCell ref="D63:E64"/>
+    <mergeCell ref="F63:G64"/>
+    <mergeCell ref="H63:I64"/>
+    <mergeCell ref="H53:I54"/>
+    <mergeCell ref="B49:C50"/>
+    <mergeCell ref="F49:G50"/>
+    <mergeCell ref="B43:C44"/>
+    <mergeCell ref="D43:E44"/>
+    <mergeCell ref="F43:G44"/>
+    <mergeCell ref="H43:I44"/>
+    <mergeCell ref="L43:M44"/>
+    <mergeCell ref="N43:O44"/>
+    <mergeCell ref="A41:O41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="L49:M50"/>
+    <mergeCell ref="J50:K51"/>
+    <mergeCell ref="D51:E52"/>
+    <mergeCell ref="H51:I52"/>
+    <mergeCell ref="L46:M47"/>
+    <mergeCell ref="L29:M30"/>
+    <mergeCell ref="J30:K31"/>
+    <mergeCell ref="D31:E32"/>
+    <mergeCell ref="H31:I32"/>
+    <mergeCell ref="J34:K35"/>
+    <mergeCell ref="D35:E36"/>
+    <mergeCell ref="H35:I36"/>
+    <mergeCell ref="D25:E26"/>
+    <mergeCell ref="H25:I26"/>
+    <mergeCell ref="J25:K27"/>
+    <mergeCell ref="D27:E28"/>
     <mergeCell ref="B29:C30"/>
     <mergeCell ref="F29:G30"/>
     <mergeCell ref="B23:C24"/>
@@ -2434,74 +2560,27 @@
     <mergeCell ref="H7:I8"/>
     <mergeCell ref="D11:E12"/>
     <mergeCell ref="F3:G4"/>
-    <mergeCell ref="L29:M30"/>
-    <mergeCell ref="J30:K31"/>
-    <mergeCell ref="D31:E32"/>
-    <mergeCell ref="H31:I32"/>
-    <mergeCell ref="J34:K35"/>
-    <mergeCell ref="D35:E36"/>
-    <mergeCell ref="H35:I36"/>
-    <mergeCell ref="D25:E26"/>
-    <mergeCell ref="H25:I26"/>
-    <mergeCell ref="J25:K27"/>
-    <mergeCell ref="D27:E28"/>
-    <mergeCell ref="H27:I28"/>
-    <mergeCell ref="B49:C50"/>
-    <mergeCell ref="F49:G50"/>
-    <mergeCell ref="B43:C44"/>
-    <mergeCell ref="D43:E44"/>
-    <mergeCell ref="F43:G44"/>
-    <mergeCell ref="H43:I44"/>
-    <mergeCell ref="L43:M44"/>
-    <mergeCell ref="N43:O44"/>
-    <mergeCell ref="A41:O41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="L49:M50"/>
-    <mergeCell ref="J50:K51"/>
-    <mergeCell ref="D51:E52"/>
-    <mergeCell ref="H51:I52"/>
-    <mergeCell ref="J54:K55"/>
-    <mergeCell ref="D55:E56"/>
-    <mergeCell ref="H55:I56"/>
-    <mergeCell ref="D45:E46"/>
-    <mergeCell ref="H45:I46"/>
-    <mergeCell ref="J45:K47"/>
-    <mergeCell ref="D47:E48"/>
-    <mergeCell ref="H47:I48"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="F69:G70"/>
-    <mergeCell ref="B63:C64"/>
-    <mergeCell ref="D63:E64"/>
-    <mergeCell ref="F63:G64"/>
-    <mergeCell ref="H63:I64"/>
-    <mergeCell ref="L63:M64"/>
-    <mergeCell ref="N63:O64"/>
-    <mergeCell ref="A61:O61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="L62:M62"/>
-    <mergeCell ref="N62:O62"/>
-    <mergeCell ref="L69:M70"/>
-    <mergeCell ref="J70:K71"/>
-    <mergeCell ref="D71:E72"/>
-    <mergeCell ref="H71:I72"/>
-    <mergeCell ref="J74:K75"/>
-    <mergeCell ref="D75:E76"/>
-    <mergeCell ref="H75:I76"/>
-    <mergeCell ref="D65:E66"/>
-    <mergeCell ref="H65:I66"/>
-    <mergeCell ref="J65:K67"/>
-    <mergeCell ref="D67:E68"/>
-    <mergeCell ref="H67:I68"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="N9:O10"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="J10:K11"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="J5:K7"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="J14:K15"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="B3:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ultima semana de planificacion, se añade una hora mas de repaso
</commit_message>
<xml_diff>
--- a/Horario.xlsx
+++ b/Horario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099B7CA0-691A-4632-852B-93026872F3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E43913-1EE6-4C0D-85F4-C336C57EAE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{5BBD8727-8E97-4145-910C-D98B6570B875}"/>
   </bookViews>
@@ -495,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -537,120 +537,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -664,6 +550,84 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -674,6 +638,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1000,111 +1006,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BDC904-63CB-49D9-B79D-E95CC9E732E1}">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46:M47"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="N63" sqref="N63:O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
     </row>
     <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A2" s="9"/>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="37" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="37" t="s">
+      <c r="E2" s="51"/>
+      <c r="F2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="37" t="s">
+      <c r="G2" s="51"/>
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="37" t="s">
+      <c r="I2" s="51"/>
+      <c r="J2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="37" t="s">
+      <c r="K2" s="51"/>
+      <c r="L2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="38"/>
-      <c r="N2" s="37" t="s">
+      <c r="M2" s="51"/>
+      <c r="N2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="38"/>
+      <c r="O2" s="51"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="41" t="s">
+      <c r="B3" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="41" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="42"/>
+      <c r="I3" s="39"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
-      <c r="L3" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="34"/>
-      <c r="N3" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="34"/>
+      <c r="L3" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="31"/>
+      <c r="N3" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="31"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="36"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="33"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
@@ -1112,20 +1118,20 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="52"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="51" t="s">
+      <c r="H5" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="52"/>
-      <c r="J5" s="41" t="s">
+      <c r="I5" s="35"/>
+      <c r="J5" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="42"/>
+      <c r="K5" s="39"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
@@ -1137,14 +1143,14 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="54"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="46"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="41"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
@@ -1156,18 +1162,18 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="56"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="55" t="s">
+      <c r="H7" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="44"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="43"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
@@ -1179,12 +1185,12 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="58"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="10"/>
@@ -1200,20 +1206,20 @@
       <c r="C9" s="15"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="48"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="14"/>
       <c r="M9" s="15"/>
-      <c r="N9" s="25" t="s">
+      <c r="N9" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="26"/>
+      <c r="O9" s="61"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
@@ -1223,18 +1229,18 @@
       <c r="C10" s="20"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="50"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="34"/>
+      <c r="J10" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="31"/>
       <c r="L10" s="16"/>
       <c r="M10" s="17"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="28"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="63"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
@@ -1242,18 +1248,18 @@
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
-      <c r="D11" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="34"/>
+      <c r="D11" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="31"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="34"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="36"/>
+      <c r="H11" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="31"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="33"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
       <c r="N11" s="10"/>
@@ -1265,12 +1271,12 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="36"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="36"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -1309,10 +1315,10 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="48"/>
+      <c r="K14" s="27"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
@@ -1322,22 +1328,22 @@
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="47" t="s">
+      <c r="C15" s="65"/>
+      <c r="D15" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="48"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="47" t="s">
+      <c r="H15" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="48"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="50"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
@@ -1347,14 +1353,14 @@
       <c r="A16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="50"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="50"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="29"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="10"/>
@@ -1396,127 +1402,127 @@
       <c r="O18" s="1"/>
     </row>
     <row r="21" spans="1:16" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
     </row>
     <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A22" s="9"/>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="37" t="s">
+      <c r="C22" s="50"/>
+      <c r="D22" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="37" t="s">
+      <c r="E22" s="51"/>
+      <c r="F22" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="38"/>
-      <c r="H22" s="37" t="s">
+      <c r="G22" s="51"/>
+      <c r="H22" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="38"/>
-      <c r="J22" s="37" t="s">
+      <c r="I22" s="51"/>
+      <c r="J22" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="K22" s="38"/>
-      <c r="L22" s="37" t="s">
+      <c r="K22" s="51"/>
+      <c r="L22" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="M22" s="38"/>
-      <c r="N22" s="37" t="s">
+      <c r="M22" s="51"/>
+      <c r="N22" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="O22" s="38"/>
+      <c r="O22" s="51"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="41" t="s">
+      <c r="B23" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="34"/>
-      <c r="H23" s="41" t="s">
+      <c r="E23" s="39"/>
+      <c r="F23" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="31"/>
+      <c r="H23" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="42"/>
+      <c r="I23" s="39"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
-      <c r="L23" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="M23" s="34"/>
-      <c r="N23" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="O23" s="34"/>
+      <c r="L23" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="31"/>
+      <c r="N23" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="O23" s="31"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="44"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="43"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="36"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="33"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="51" t="s">
+      <c r="C25" s="57"/>
+      <c r="D25" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="52"/>
+      <c r="E25" s="35"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="51" t="s">
+      <c r="H25" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="52"/>
-      <c r="J25" s="41" t="s">
+      <c r="I25" s="35"/>
+      <c r="J25" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="K25" s="42"/>
+      <c r="K25" s="39"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
@@ -1526,16 +1532,16 @@
       <c r="A26" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="54"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="37"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="46"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="41"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
@@ -1547,18 +1553,18 @@
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="56"/>
+      <c r="E27" s="45"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="60" t="s">
+      <c r="H27" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I27" s="63"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="44"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="43"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
@@ -1570,12 +1576,12 @@
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="58"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="47"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="59"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="21"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="10"/>
@@ -1587,24 +1593,24 @@
       <c r="A29" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="48"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
-      <c r="F29" s="47" t="s">
+      <c r="F29" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="48"/>
-      <c r="H29" s="61"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="23"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
-      <c r="L29" s="47" t="s">
+      <c r="L29" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="48"/>
+      <c r="M29" s="27"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
     </row>
@@ -1612,20 +1618,20 @@
       <c r="A30" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="49"/>
-      <c r="C30" s="50"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="50"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
-      <c r="J30" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="K30" s="34"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="50"/>
+      <c r="J30" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K30" s="31"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="29"/>
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
     </row>
@@ -1635,18 +1641,18 @@
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
-      <c r="D31" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="34"/>
+      <c r="D31" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="31"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
-      <c r="H31" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="I31" s="34"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="36"/>
+      <c r="H31" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" s="31"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="33"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
       <c r="N31" s="10"/>
@@ -1658,12 +1664,12 @@
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="36"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="33"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="36"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="33"/>
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
       <c r="L32" s="10"/>
@@ -1702,10 +1708,10 @@
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
-      <c r="J34" s="47" t="s">
+      <c r="J34" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K34" s="48"/>
+      <c r="K34" s="27"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
@@ -1717,18 +1723,18 @@
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
-      <c r="D35" s="47" t="s">
+      <c r="D35" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="48"/>
+      <c r="E35" s="27"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
-      <c r="H35" s="47" t="s">
+      <c r="H35" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I35" s="48"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="50"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="29"/>
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
@@ -1740,12 +1746,12 @@
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="50"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="29"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="50"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="29"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="10"/>
@@ -1754,104 +1760,104 @@
       <c r="O36" s="10"/>
     </row>
     <row r="41" spans="1:15" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
-      <c r="M41" s="39"/>
-      <c r="N41" s="39"/>
-      <c r="O41" s="39"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="48"/>
+      <c r="O41" s="48"/>
     </row>
     <row r="42" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A42" s="9"/>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="40"/>
-      <c r="D42" s="37" t="s">
+      <c r="C42" s="50"/>
+      <c r="D42" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="37" t="s">
+      <c r="E42" s="51"/>
+      <c r="F42" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="G42" s="38"/>
-      <c r="H42" s="37" t="s">
+      <c r="G42" s="51"/>
+      <c r="H42" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I42" s="38"/>
-      <c r="J42" s="37" t="s">
+      <c r="I42" s="51"/>
+      <c r="J42" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="K42" s="38"/>
-      <c r="L42" s="37" t="s">
+      <c r="K42" s="51"/>
+      <c r="L42" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="M42" s="38"/>
-      <c r="N42" s="37" t="s">
+      <c r="M42" s="51"/>
+      <c r="N42" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="O42" s="38"/>
+      <c r="O42" s="51"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="34"/>
-      <c r="D43" s="41" t="s">
+      <c r="B43" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="31"/>
+      <c r="D43" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="42"/>
-      <c r="F43" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="G43" s="34"/>
-      <c r="H43" s="41" t="s">
+      <c r="E43" s="39"/>
+      <c r="F43" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="31"/>
+      <c r="H43" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="I43" s="42"/>
+      <c r="I43" s="39"/>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
-      <c r="L43" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="M43" s="34"/>
-      <c r="N43" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="O43" s="34"/>
+      <c r="L43" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="M43" s="31"/>
+      <c r="N43" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="O43" s="31"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="35"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="44"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="43"/>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="36"/>
-      <c r="N44" s="35"/>
-      <c r="O44" s="36"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="33"/>
+      <c r="N44" s="32"/>
+      <c r="O44" s="33"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
@@ -1859,20 +1865,20 @@
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
-      <c r="D45" s="51" t="s">
+      <c r="D45" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="E45" s="52"/>
+      <c r="E45" s="35"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="51" t="s">
+      <c r="H45" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="I45" s="52"/>
-      <c r="J45" s="41" t="s">
+      <c r="I45" s="35"/>
+      <c r="J45" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="K45" s="42"/>
+      <c r="K45" s="39"/>
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
@@ -1884,18 +1890,18 @@
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="54"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="37"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="54"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="64" t="s">
+      <c r="H46" s="36"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="M46" s="65"/>
+      <c r="M46" s="53"/>
       <c r="N46" s="10"/>
       <c r="O46" s="10"/>
     </row>
@@ -1905,20 +1911,20 @@
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
-      <c r="D47" s="55" t="s">
+      <c r="D47" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="E47" s="56"/>
+      <c r="E47" s="45"/>
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
-      <c r="H47" s="55" t="s">
+      <c r="H47" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="I47" s="56"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="44"/>
-      <c r="L47" s="66"/>
-      <c r="M47" s="67"/>
+      <c r="I47" s="45"/>
+      <c r="J47" s="42"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="55"/>
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
     </row>
@@ -1928,12 +1934,12 @@
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="58"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="47"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
-      <c r="H48" s="57"/>
-      <c r="I48" s="58"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="47"/>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="10"/>
@@ -1945,24 +1951,24 @@
       <c r="A49" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="47" t="s">
+      <c r="B49" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="48"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
-      <c r="F49" s="47" t="s">
+      <c r="F49" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G49" s="48"/>
+      <c r="G49" s="27"/>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
-      <c r="L49" s="47" t="s">
+      <c r="L49" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M49" s="48"/>
+      <c r="M49" s="27"/>
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
     </row>
@@ -1970,20 +1976,20 @@
       <c r="A50" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="49"/>
-      <c r="C50" s="50"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="29"/>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="50"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="29"/>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
-      <c r="J50" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="K50" s="34"/>
-      <c r="L50" s="49"/>
-      <c r="M50" s="50"/>
+      <c r="J50" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K50" s="31"/>
+      <c r="L50" s="28"/>
+      <c r="M50" s="29"/>
       <c r="N50" s="10"/>
       <c r="O50" s="10"/>
     </row>
@@ -1993,18 +1999,18 @@
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
-      <c r="D51" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="34"/>
+      <c r="D51" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" s="31"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
-      <c r="H51" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="I51" s="34"/>
-      <c r="J51" s="35"/>
-      <c r="K51" s="36"/>
+      <c r="H51" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I51" s="31"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="33"/>
       <c r="L51" s="12"/>
       <c r="M51" s="12"/>
       <c r="N51" s="10"/>
@@ -2016,12 +2022,12 @@
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="36"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="33"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="36"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="33"/>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
@@ -2039,10 +2045,10 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
-      <c r="H53" s="51" t="s">
+      <c r="H53" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="I53" s="52"/>
+      <c r="I53" s="35"/>
       <c r="J53" s="10"/>
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
@@ -2060,12 +2066,12 @@
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
-      <c r="H54" s="53"/>
-      <c r="I54" s="54"/>
-      <c r="J54" s="47" t="s">
+      <c r="H54" s="36"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K54" s="48"/>
+      <c r="K54" s="27"/>
       <c r="L54" s="10"/>
       <c r="M54" s="10"/>
       <c r="N54" s="10"/>
@@ -2077,18 +2083,18 @@
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
-      <c r="D55" s="47" t="s">
+      <c r="D55" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="48"/>
+      <c r="E55" s="27"/>
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
-      <c r="H55" s="47" t="s">
+      <c r="H55" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I55" s="48"/>
-      <c r="J55" s="49"/>
-      <c r="K55" s="50"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="28"/>
+      <c r="K55" s="29"/>
       <c r="L55" s="10"/>
       <c r="M55" s="10"/>
       <c r="N55" s="10"/>
@@ -2100,12 +2106,12 @@
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="50"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="29"/>
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
-      <c r="H56" s="49"/>
-      <c r="I56" s="50"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="29"/>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="10"/>
@@ -2114,129 +2120,129 @@
       <c r="O56" s="10"/>
     </row>
     <row r="61" spans="1:15" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A61" s="39" t="s">
+      <c r="A61" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
-      <c r="I61" s="39"/>
-      <c r="J61" s="39"/>
-      <c r="K61" s="39"/>
-      <c r="L61" s="39"/>
-      <c r="M61" s="39"/>
-      <c r="N61" s="39"/>
-      <c r="O61" s="39"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="48"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="48"/>
+      <c r="L61" s="48"/>
+      <c r="M61" s="48"/>
+      <c r="N61" s="48"/>
+      <c r="O61" s="48"/>
     </row>
     <row r="62" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A62" s="9"/>
-      <c r="B62" s="37" t="s">
+      <c r="B62" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="40"/>
-      <c r="D62" s="37" t="s">
+      <c r="C62" s="50"/>
+      <c r="D62" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="38"/>
-      <c r="F62" s="37" t="s">
+      <c r="E62" s="51"/>
+      <c r="F62" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="G62" s="38"/>
-      <c r="H62" s="37" t="s">
+      <c r="G62" s="51"/>
+      <c r="H62" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I62" s="38"/>
-      <c r="J62" s="37" t="s">
+      <c r="I62" s="51"/>
+      <c r="J62" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="K62" s="38"/>
-      <c r="L62" s="37" t="s">
+      <c r="K62" s="51"/>
+      <c r="L62" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="M62" s="38"/>
-      <c r="N62" s="37" t="s">
+      <c r="M62" s="51"/>
+      <c r="N62" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="O62" s="38"/>
+      <c r="O62" s="51"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B63" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="34"/>
-      <c r="D63" s="41" t="s">
+      <c r="B63" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="31"/>
+      <c r="D63" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="E63" s="42"/>
-      <c r="F63" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="G63" s="34"/>
-      <c r="H63" s="41" t="s">
+      <c r="E63" s="39"/>
+      <c r="F63" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G63" s="31"/>
+      <c r="H63" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="I63" s="42"/>
+      <c r="I63" s="39"/>
       <c r="J63" s="10"/>
       <c r="K63" s="10"/>
-      <c r="L63" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="M63" s="34"/>
-      <c r="N63" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="O63" s="34"/>
+      <c r="L63" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="M63" s="31"/>
+      <c r="N63" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="O63" s="31"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B64" s="35"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="44"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="36"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="44"/>
+      <c r="B64" s="68"/>
+      <c r="C64" s="69"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="69"/>
+      <c r="H64" s="42"/>
+      <c r="I64" s="43"/>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
-      <c r="L64" s="35"/>
-      <c r="M64" s="36"/>
-      <c r="N64" s="35"/>
-      <c r="O64" s="36"/>
+      <c r="L64" s="68"/>
+      <c r="M64" s="69"/>
+      <c r="N64" s="68"/>
+      <c r="O64" s="69"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="51" t="s">
+      <c r="B65" s="32"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="E65" s="52"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="10"/>
-      <c r="H65" s="51" t="s">
+      <c r="E65" s="35"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="33"/>
+      <c r="H65" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="I65" s="52"/>
-      <c r="J65" s="41" t="s">
+      <c r="I65" s="35"/>
+      <c r="J65" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="K65" s="42"/>
-      <c r="L65" s="10"/>
-      <c r="M65" s="10"/>
-      <c r="N65" s="10"/>
-      <c r="O65" s="10"/>
+      <c r="K65" s="39"/>
+      <c r="L65" s="32"/>
+      <c r="M65" s="33"/>
+      <c r="N65" s="32"/>
+      <c r="O65" s="33"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
@@ -2244,14 +2250,14 @@
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
-      <c r="D66" s="53"/>
-      <c r="E66" s="54"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="37"/>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
-      <c r="H66" s="53"/>
-      <c r="I66" s="54"/>
-      <c r="J66" s="45"/>
-      <c r="K66" s="46"/>
+      <c r="H66" s="36"/>
+      <c r="I66" s="37"/>
+      <c r="J66" s="40"/>
+      <c r="K66" s="41"/>
       <c r="L66" s="10"/>
       <c r="M66" s="10"/>
       <c r="N66" s="10"/>
@@ -2263,15 +2269,15 @@
       </c>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
-      <c r="D67" s="55" t="s">
+      <c r="D67" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="E67" s="56"/>
+      <c r="E67" s="45"/>
       <c r="F67" s="10"/>
       <c r="G67" s="14"/>
       <c r="I67" s="15"/>
-      <c r="J67" s="43"/>
-      <c r="K67" s="44"/>
+      <c r="J67" s="42"/>
+      <c r="K67" s="43"/>
       <c r="L67" s="10"/>
       <c r="M67" s="10"/>
       <c r="N67" s="10"/>
@@ -2283,8 +2289,8 @@
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
-      <c r="D68" s="57"/>
-      <c r="E68" s="58"/>
+      <c r="D68" s="46"/>
+      <c r="E68" s="47"/>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
       <c r="H68" s="16"/>
@@ -2300,24 +2306,24 @@
       <c r="A69" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B69" s="47" t="s">
+      <c r="B69" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C69" s="48"/>
+      <c r="C69" s="27"/>
       <c r="D69" s="10"/>
       <c r="E69" s="10"/>
-      <c r="F69" s="47" t="s">
+      <c r="F69" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G69" s="48"/>
+      <c r="G69" s="27"/>
       <c r="H69" s="10"/>
       <c r="I69" s="10"/>
       <c r="J69" s="10"/>
       <c r="K69" s="10"/>
-      <c r="L69" s="47" t="s">
+      <c r="L69" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M69" s="48"/>
+      <c r="M69" s="27"/>
       <c r="N69" s="10"/>
       <c r="O69" s="10"/>
     </row>
@@ -2325,20 +2331,20 @@
       <c r="A70" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B70" s="49"/>
-      <c r="C70" s="50"/>
+      <c r="B70" s="28"/>
+      <c r="C70" s="29"/>
       <c r="D70" s="10"/>
       <c r="E70" s="10"/>
-      <c r="F70" s="49"/>
-      <c r="G70" s="50"/>
+      <c r="F70" s="28"/>
+      <c r="G70" s="29"/>
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
-      <c r="J70" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="K70" s="34"/>
-      <c r="L70" s="49"/>
-      <c r="M70" s="50"/>
+      <c r="J70" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K70" s="31"/>
+      <c r="L70" s="28"/>
+      <c r="M70" s="29"/>
       <c r="N70" s="10"/>
       <c r="O70" s="10"/>
     </row>
@@ -2348,18 +2354,18 @@
       </c>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
-      <c r="D71" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E71" s="34"/>
+      <c r="D71" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" s="31"/>
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
-      <c r="H71" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="I71" s="34"/>
-      <c r="J71" s="35"/>
-      <c r="K71" s="36"/>
+      <c r="H71" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I71" s="31"/>
+      <c r="J71" s="68"/>
+      <c r="K71" s="69"/>
       <c r="L71" s="12"/>
       <c r="M71" s="12"/>
       <c r="N71" s="10"/>
@@ -2371,14 +2377,14 @@
       </c>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="36"/>
+      <c r="D72" s="68"/>
+      <c r="E72" s="69"/>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
-      <c r="H72" s="35"/>
-      <c r="I72" s="36"/>
-      <c r="J72" s="10"/>
-      <c r="K72" s="10"/>
+      <c r="H72" s="68"/>
+      <c r="I72" s="69"/>
+      <c r="J72" s="32"/>
+      <c r="K72" s="33"/>
       <c r="L72" s="10"/>
       <c r="M72" s="10"/>
       <c r="N72" s="10"/>
@@ -2390,12 +2396,12 @@
       </c>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="33"/>
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
-      <c r="H73" s="10"/>
-      <c r="I73" s="10"/>
+      <c r="H73" s="32"/>
+      <c r="I73" s="33"/>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
       <c r="L73" s="10"/>
@@ -2415,10 +2421,10 @@
       <c r="G74" s="10"/>
       <c r="H74" s="10"/>
       <c r="I74" s="10"/>
-      <c r="J74" s="47" t="s">
+      <c r="J74" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K74" s="48"/>
+      <c r="K74" s="27"/>
       <c r="L74" s="10"/>
       <c r="M74" s="10"/>
       <c r="N74" s="10"/>
@@ -2430,18 +2436,18 @@
       </c>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
-      <c r="D75" s="47" t="s">
+      <c r="D75" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="48"/>
+      <c r="E75" s="27"/>
       <c r="F75" s="11"/>
       <c r="G75" s="11"/>
-      <c r="H75" s="47" t="s">
+      <c r="H75" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I75" s="48"/>
-      <c r="J75" s="49"/>
-      <c r="K75" s="50"/>
+      <c r="I75" s="27"/>
+      <c r="J75" s="28"/>
+      <c r="K75" s="29"/>
       <c r="L75" s="10"/>
       <c r="M75" s="10"/>
       <c r="N75" s="10"/>
@@ -2453,12 +2459,12 @@
       </c>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
-      <c r="D76" s="49"/>
-      <c r="E76" s="50"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="29"/>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
-      <c r="H76" s="49"/>
-      <c r="I76" s="50"/>
+      <c r="H76" s="28"/>
+      <c r="I76" s="29"/>
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
       <c r="L76" s="10"/>
@@ -2468,80 +2474,20 @@
     </row>
   </sheetData>
   <mergeCells count="113">
-    <mergeCell ref="L69:M70"/>
-    <mergeCell ref="J70:K71"/>
-    <mergeCell ref="D71:E72"/>
-    <mergeCell ref="H71:I72"/>
-    <mergeCell ref="J74:K75"/>
-    <mergeCell ref="D75:E76"/>
-    <mergeCell ref="H75:I76"/>
-    <mergeCell ref="D65:E66"/>
-    <mergeCell ref="H65:I66"/>
-    <mergeCell ref="J65:K67"/>
-    <mergeCell ref="D67:E68"/>
-    <mergeCell ref="L63:M64"/>
-    <mergeCell ref="N63:O64"/>
-    <mergeCell ref="A61:O61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="L62:M62"/>
-    <mergeCell ref="N62:O62"/>
-    <mergeCell ref="J54:K55"/>
-    <mergeCell ref="D55:E56"/>
-    <mergeCell ref="H55:I56"/>
-    <mergeCell ref="D45:E46"/>
-    <mergeCell ref="H45:I46"/>
-    <mergeCell ref="J45:K47"/>
-    <mergeCell ref="D47:E48"/>
-    <mergeCell ref="H47:I48"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="F69:G70"/>
-    <mergeCell ref="B63:C64"/>
-    <mergeCell ref="D63:E64"/>
-    <mergeCell ref="F63:G64"/>
-    <mergeCell ref="H63:I64"/>
-    <mergeCell ref="H53:I54"/>
-    <mergeCell ref="B49:C50"/>
-    <mergeCell ref="F49:G50"/>
-    <mergeCell ref="B43:C44"/>
-    <mergeCell ref="D43:E44"/>
-    <mergeCell ref="F43:G44"/>
-    <mergeCell ref="H43:I44"/>
-    <mergeCell ref="L43:M44"/>
-    <mergeCell ref="N43:O44"/>
-    <mergeCell ref="A41:O41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="L49:M50"/>
-    <mergeCell ref="J50:K51"/>
-    <mergeCell ref="D51:E52"/>
-    <mergeCell ref="H51:I52"/>
-    <mergeCell ref="L46:M47"/>
-    <mergeCell ref="L29:M30"/>
-    <mergeCell ref="J30:K31"/>
-    <mergeCell ref="D31:E32"/>
-    <mergeCell ref="H31:I32"/>
-    <mergeCell ref="J34:K35"/>
-    <mergeCell ref="D35:E36"/>
-    <mergeCell ref="H35:I36"/>
-    <mergeCell ref="D25:E26"/>
-    <mergeCell ref="H25:I26"/>
-    <mergeCell ref="J25:K27"/>
-    <mergeCell ref="D27:E28"/>
-    <mergeCell ref="B29:C30"/>
-    <mergeCell ref="F29:G30"/>
-    <mergeCell ref="B23:C24"/>
-    <mergeCell ref="D23:E24"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="H23:I24"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="J5:K7"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="B3:C4"/>
     <mergeCell ref="L23:M24"/>
     <mergeCell ref="N23:O24"/>
     <mergeCell ref="L3:M4"/>
@@ -2560,27 +2506,87 @@
     <mergeCell ref="H7:I8"/>
     <mergeCell ref="D11:E12"/>
     <mergeCell ref="F3:G4"/>
-    <mergeCell ref="B25:C26"/>
     <mergeCell ref="N9:O10"/>
     <mergeCell ref="B15:C16"/>
     <mergeCell ref="J10:K11"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="H11:I12"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="J5:K7"/>
     <mergeCell ref="D15:E16"/>
     <mergeCell ref="H15:I16"/>
     <mergeCell ref="J14:K15"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D25:E26"/>
+    <mergeCell ref="H25:I26"/>
+    <mergeCell ref="J25:K27"/>
+    <mergeCell ref="D27:E28"/>
+    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="F29:G30"/>
+    <mergeCell ref="B23:C24"/>
+    <mergeCell ref="D23:E24"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="H23:I24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="L49:M50"/>
+    <mergeCell ref="J50:K51"/>
+    <mergeCell ref="D51:E52"/>
+    <mergeCell ref="H51:I52"/>
+    <mergeCell ref="L46:M47"/>
+    <mergeCell ref="L29:M30"/>
+    <mergeCell ref="J30:K31"/>
+    <mergeCell ref="D31:E32"/>
+    <mergeCell ref="H31:I32"/>
+    <mergeCell ref="J34:K35"/>
+    <mergeCell ref="D35:E36"/>
+    <mergeCell ref="H35:I36"/>
+    <mergeCell ref="B43:C44"/>
+    <mergeCell ref="D43:E44"/>
+    <mergeCell ref="F43:G44"/>
+    <mergeCell ref="H43:I44"/>
+    <mergeCell ref="L43:M44"/>
+    <mergeCell ref="N43:O44"/>
+    <mergeCell ref="A41:O41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="J54:K55"/>
+    <mergeCell ref="D55:E56"/>
+    <mergeCell ref="H55:I56"/>
+    <mergeCell ref="D45:E46"/>
+    <mergeCell ref="H45:I46"/>
+    <mergeCell ref="J45:K47"/>
+    <mergeCell ref="D47:E48"/>
+    <mergeCell ref="H47:I48"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="F69:G70"/>
+    <mergeCell ref="D63:E64"/>
+    <mergeCell ref="H63:I64"/>
+    <mergeCell ref="H53:I54"/>
+    <mergeCell ref="B49:C50"/>
+    <mergeCell ref="F49:G50"/>
+    <mergeCell ref="B63:C65"/>
+    <mergeCell ref="F63:G65"/>
+    <mergeCell ref="J70:K72"/>
+    <mergeCell ref="A61:O61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="L63:M65"/>
+    <mergeCell ref="N63:O65"/>
+    <mergeCell ref="L69:M70"/>
+    <mergeCell ref="J74:K75"/>
+    <mergeCell ref="D75:E76"/>
+    <mergeCell ref="H75:I76"/>
+    <mergeCell ref="D65:E66"/>
+    <mergeCell ref="H65:I66"/>
+    <mergeCell ref="J65:K67"/>
+    <mergeCell ref="D67:E68"/>
+    <mergeCell ref="D71:E73"/>
+    <mergeCell ref="H71:I73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>